<commit_message>
Completed original office scene
</commit_message>
<xml_diff>
--- a/ObjectsInLocations.xlsx
+++ b/ObjectsInLocations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30615" windowHeight="14265"/>
+    <workbookView windowWidth="28695" windowHeight="13185"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,10 +534,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -549,6 +549,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -556,22 +563,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -587,9 +579,33 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -601,9 +617,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -617,6 +632,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -625,23 +648,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -663,30 +671,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -707,7 +707,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,163 +881,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,17 +898,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -937,6 +926,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -951,17 +955,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -983,18 +990,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,7 +1003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1021,130 +1021,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1479,8 +1479,8 @@
   <sheetPr/>
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2579,8 +2579,7 @@
         <v>11</v>
       </c>
       <c r="G45">
-        <f>D48</f>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H45" t="s">
         <v>11</v>
@@ -2602,9 +2601,8 @@
       <c r="F46" t="s">
         <v>11</v>
       </c>
-      <c r="G46">
-        <f>D45</f>
-        <v>43</v>
+      <c r="G46" t="s">
+        <v>11</v>
       </c>
       <c r="H46" t="s">
         <v>11</v>
@@ -2656,7 +2654,6 @@
         <v>11</v>
       </c>
       <c r="G48">
-        <f>D37</f>
         <v>35</v>
       </c>
       <c r="H48" t="s">

</xml_diff>

<commit_message>
Put together the rest of the scenes
</commit_message>
<xml_diff>
--- a/ObjectsInLocations.xlsx
+++ b/ObjectsInLocations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185"/>
+    <workbookView windowWidth="24150" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -563,6 +563,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -585,9 +600,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -618,7 +632,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -626,7 +640,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -648,6 +662,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -662,31 +685,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -707,7 +707,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -719,13 +785,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,19 +803,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,43 +833,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,31 +863,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,43 +881,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,6 +898,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -925,6 +936,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -940,35 +960,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -988,13 +984,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1021,130 +1021,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1479,8 +1479,8 @@
   <sheetPr/>
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Put scenes in order
</commit_message>
<xml_diff>
--- a/ObjectsInLocations.xlsx
+++ b/ObjectsInLocations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24150" windowHeight="12630"/>
+    <workbookView windowWidth="30615" windowHeight="14265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172">
   <si>
     <t>Location ID</t>
   </si>
@@ -491,6 +491,9 @@
   </si>
   <si>
     <t>Those screws will need to come off if I'm to fix the lift.</t>
+  </si>
+  <si>
+    <t>NOW THE PUZZLE FOR PUTTING THE PIN TOGETHER</t>
   </si>
   <si>
     <t>The panel to cover up the lift's innards.</t>
@@ -549,21 +552,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -571,7 +560,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,16 +581,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -612,6 +593,38 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -632,31 +645,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -670,9 +659,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -685,6 +673,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -692,7 +695,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -707,19 +710,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,43 +824,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,13 +866,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,91 +884,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -903,10 +912,32 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -916,7 +947,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -936,15 +967,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -956,15 +978,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -984,17 +997,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,7 +1012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1021,139 +1030,145 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
@@ -1479,8 +1494,8 @@
   <sheetPr/>
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1619,7 +1634,7 @@
       <c r="H5" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3465,125 +3480,131 @@
       <c r="A84">
         <v>12</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="2">
         <v>82</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="2">
         <f>D88</f>
         <v>86</v>
       </c>
-      <c r="F84" t="s">
-        <v>11</v>
-      </c>
-      <c r="G84">
+      <c r="F84" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" s="2">
         <f>D31</f>
         <v>29</v>
       </c>
-      <c r="H84" t="s">
-        <v>11</v>
-      </c>
-      <c r="I84" t="s">
+      <c r="H84" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I84" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="85" spans="3:9">
-      <c r="C85" t="s">
+    <row r="85" ht="30" spans="2:9">
+      <c r="B85" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="2">
         <v>83</v>
       </c>
-      <c r="E85" t="s">
-        <v>11</v>
-      </c>
-      <c r="F85" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85">
+      <c r="E85" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="2">
         <f>D88</f>
         <v>86</v>
       </c>
-      <c r="H85" t="s">
-        <v>11</v>
-      </c>
-      <c r="I85" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="86" spans="3:9">
-      <c r="C86" t="s">
+      <c r="H85" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I85" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D86">
+    </row>
+    <row r="86" spans="2:9">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D86" s="2">
         <v>84</v>
       </c>
-      <c r="E86" t="s">
-        <v>11</v>
-      </c>
-      <c r="F86" t="s">
-        <v>11</v>
-      </c>
-      <c r="G86" t="s">
-        <v>11</v>
-      </c>
-      <c r="H86" t="s">
-        <v>11</v>
-      </c>
-      <c r="I86" t="s">
+      <c r="E86" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I86" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="87" spans="3:9">
-      <c r="C87" t="s">
-        <v>161</v>
-      </c>
-      <c r="D87">
+    <row r="87" spans="2:9">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D87" s="2">
         <v>85</v>
       </c>
-      <c r="E87" t="s">
-        <v>11</v>
-      </c>
-      <c r="F87" t="s">
-        <v>11</v>
-      </c>
-      <c r="G87">
+      <c r="E87" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G87" s="2">
         <f>D23</f>
         <v>21</v>
       </c>
-      <c r="H87" t="s">
-        <v>11</v>
-      </c>
-      <c r="I87" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="88" spans="3:9">
-      <c r="C88" t="s">
+      <c r="H87" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I87" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D88">
+    </row>
+    <row r="88" spans="2:9">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D88" s="2">
         <v>86</v>
       </c>
-      <c r="E88" t="s">
-        <v>11</v>
-      </c>
-      <c r="F88" t="s">
-        <v>11</v>
-      </c>
-      <c r="G88" t="s">
-        <v>11</v>
-      </c>
-      <c r="H88" t="s">
-        <v>11</v>
-      </c>
-      <c r="I88" t="s">
-        <v>164</v>
+      <c r="E88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3591,10 +3612,10 @@
         <v>13</v>
       </c>
       <c r="B89" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C89" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D89">
         <v>87</v>
@@ -3620,7 +3641,7 @@
         <v>14</v>
       </c>
       <c r="B90" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>78</v>
@@ -3641,12 +3662,12 @@
         <v>11</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" spans="3:9">
       <c r="C91" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D91">
         <v>89</v>
@@ -3665,7 +3686,7 @@
         <v>11</v>
       </c>
       <c r="I91" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>